<commit_message>
Minor docsite fixes (#309)
</commit_message>
<xml_diff>
--- a/docs/docs/arch-diagram.xlsx
+++ b/docs/docs/arch-diagram.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Corda/conclave2/docs/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Corda/conclave/docs/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8C80F5-7FE4-3244-9FEE-C9BDA2DF23B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727A62A4-B24E-384E-9DB7-1E5A07549407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-7340" windowWidth="51200" windowHeight="28340" xr2:uid="{2ED672D7-C865-D444-BDEA-C0A5C51D3721}"/>
   </bookViews>
@@ -119,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -146,32 +146,6 @@
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FFB2B2B2"/>
       </right>
@@ -257,7 +231,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,25 +245,25 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
@@ -304,13 +278,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1050,7 +1018,7 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="376" zoomScaleNormal="376" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1059,75 +1027,75 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="11"/>
+      <c r="F3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="18"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="E6" s="10" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="E6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="9" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="E6:F7"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="B3:C8"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>